<commit_message>
feat: add import employees feature
</commit_message>
<xml_diff>
--- a/API/wwwroot/examples/import-employees-example.xlsx
+++ b/API/wwwroot/examples/import-employees-example.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Febrianto\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C633387-63E9-4FB9-BF88-22CD1AD2C57D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F874B71-1A88-4361-AABD-E818B4EBD71B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3600" yWindow="3180" windowWidth="21600" windowHeight="11385" xr2:uid="{BEB39963-AECC-48B4-8D6B-4A7D2ADAF613}"/>
   </bookViews>
@@ -458,7 +458,7 @@
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -537,7 +537,7 @@
         <v>36606</v>
       </c>
       <c r="E3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F3" s="1">
         <v>45123</v>
@@ -563,7 +563,7 @@
         <v>36193</v>
       </c>
       <c r="E4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F4" s="1">
         <v>45092</v>

</xml_diff>